<commit_message>
feat: redesign the modal
</commit_message>
<xml_diff>
--- a/upload/temp/format_import_guru.xlsx
+++ b/upload/temp/format_import_guru.xlsx
@@ -25,16 +25,16 @@
     <t xml:space="preserve">format_download_verified_ok</t>
   </si>
   <si>
-    <t xml:space="preserve">no_induk</t>
+    <t xml:space="preserve">kode</t>
   </si>
   <si>
     <t xml:space="preserve">nama</t>
   </si>
   <si>
-    <t xml:space="preserve">ANTON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UJANG</t>
+    <t xml:space="preserve">sdfsdf234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfsdf234sdfsdfsdf</t>
   </si>
 </sst>
 </file>
@@ -110,12 +110,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,43 +320,43 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="16384" min="4" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="16384" min="4" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2203</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>2204</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>